<commit_message>
fixed capitalized precinct column
</commit_message>
<xml_diff>
--- a/MI_Wexford/MI_Wexford_GE20_cleaned.xlsx
+++ b/MI_Wexford/MI_Wexford_GE20_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\MI_Wexford\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835465C9-3358-4121-BF93-1EB58F9B85A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35C0FA2-54EF-4DF4-A0BC-B0FFEBD2F4D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="440" windowWidth="32510" windowHeight="18130" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19700" yWindow="1560" windowWidth="17340" windowHeight="18130" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total_reg_and_cast" sheetId="2" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="59">
-  <si>
-    <t>Precinct</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="58">
   <si>
     <t>City of Cadillac, Precinct 1</t>
   </si>
@@ -596,18 +593,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>2769</v>
@@ -618,7 +615,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2653</v>
@@ -629,7 +626,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2575</v>
@@ -640,7 +637,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>966</v>
@@ -651,7 +648,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>759</v>
@@ -662,7 +659,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>554</v>
@@ -673,7 +670,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1387</v>
@@ -684,7 +681,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2162</v>
@@ -695,7 +692,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>2139</v>
@@ -706,7 +703,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>696</v>
@@ -717,7 +714,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>493</v>
@@ -728,7 +725,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1401</v>
@@ -739,7 +736,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2881</v>
@@ -750,7 +747,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>171</v>
@@ -761,7 +758,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>705</v>
@@ -772,7 +769,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1973</v>
@@ -783,7 +780,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>482</v>
@@ -794,7 +791,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>313</v>
@@ -805,7 +802,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>1481</v>
@@ -816,7 +813,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>973</v>
@@ -827,7 +824,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -838,7 +835,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>619</v>
@@ -849,7 +846,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -860,7 +857,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>360</v>
@@ -871,7 +868,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -882,7 +879,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>256</v>
@@ -893,7 +890,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>178</v>
@@ -904,7 +901,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>302</v>
@@ -915,7 +912,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>335</v>
@@ -926,7 +923,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>33</v>
@@ -962,33 +959,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>282</v>
@@ -1014,7 +1011,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>335</v>
@@ -1040,7 +1037,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>294</v>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>82</v>
@@ -1092,7 +1089,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>85</v>
@@ -1118,7 +1115,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>54</v>
@@ -1144,7 +1141,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>101</v>
@@ -1170,7 +1167,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>212</v>
@@ -1196,7 +1193,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>191</v>
@@ -1222,7 +1219,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>81</v>
@@ -1248,7 +1245,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>40</v>
@@ -1274,7 +1271,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>136</v>
@@ -1300,7 +1297,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>252</v>
@@ -1326,7 +1323,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>22</v>
@@ -1352,7 +1349,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>38</v>
@@ -1378,7 +1375,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>161</v>
@@ -1404,7 +1401,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>51</v>
@@ -1430,7 +1427,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>36</v>
@@ -1456,7 +1453,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>115</v>
@@ -1482,7 +1479,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>75</v>
@@ -1508,7 +1505,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1534,7 +1531,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1560,7 +1557,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1586,7 +1583,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1612,7 +1609,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1638,7 +1635,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1664,7 +1661,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1690,7 +1687,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1716,7 +1713,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1742,7 +1739,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1793,33 +1790,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>600</v>
@@ -1845,7 +1842,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>652</v>
@@ -1871,7 +1868,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>659</v>
@@ -1897,7 +1894,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>162</v>
@@ -1923,7 +1920,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>149</v>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>122</v>
@@ -1975,7 +1972,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>236</v>
@@ -2001,7 +1998,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>584</v>
@@ -2027,7 +2024,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>519</v>
@@ -2053,7 +2050,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>148</v>
@@ -2079,7 +2076,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>90</v>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>268</v>
@@ -2131,7 +2128,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>542</v>
@@ -2157,7 +2154,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>36</v>
@@ -2183,7 +2180,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>100</v>
@@ -2209,7 +2206,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>386</v>
@@ -2235,7 +2232,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>106</v>
@@ -2261,7 +2258,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>81</v>
@@ -2287,7 +2284,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>232</v>
@@ -2313,7 +2310,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>166</v>
@@ -2363,30 +2360,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>589</v>
@@ -2409,7 +2406,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>657</v>
@@ -2432,7 +2429,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>636</v>
@@ -2455,7 +2452,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>160</v>
@@ -2478,7 +2475,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>156</v>
@@ -2501,7 +2498,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>126</v>
@@ -2524,7 +2521,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>244</v>
@@ -2547,7 +2544,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>552</v>
@@ -2570,7 +2567,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>489</v>
@@ -2593,7 +2590,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>140</v>
@@ -2616,7 +2613,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>89</v>
@@ -2639,7 +2636,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>251</v>
@@ -2662,7 +2659,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>518</v>
@@ -2685,7 +2682,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>35</v>
@@ -2708,7 +2705,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>97</v>
@@ -2731,7 +2728,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>371</v>
@@ -2754,7 +2751,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>101</v>
@@ -2777,7 +2774,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>81</v>
@@ -2800,7 +2797,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>229</v>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>163</v>
@@ -2853,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C6B455-39A4-44C6-8973-49D39175A8D5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2869,27 +2866,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>523</v>
@@ -2909,7 +2906,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>573</v>
@@ -2929,7 +2926,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>546</v>
@@ -2949,7 +2946,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>143</v>
@@ -2969,7 +2966,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>133</v>
@@ -2989,7 +2986,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>101</v>
@@ -3009,7 +3006,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>212</v>
@@ -3029,7 +3026,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>474</v>
@@ -3049,7 +3046,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>434</v>
@@ -3069,7 +3066,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>116</v>
@@ -3089,7 +3086,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>78</v>
@@ -3109,7 +3106,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>239</v>
@@ -3129,7 +3126,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>458</v>
@@ -3149,7 +3146,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>32</v>
@@ -3169,7 +3166,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>83</v>
@@ -3189,7 +3186,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>326</v>
@@ -3209,7 +3206,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>83</v>
@@ -3229,7 +3226,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>75</v>
@@ -3249,7 +3246,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>206</v>
@@ -3269,7 +3266,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>138</v>
@@ -3296,7 +3293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBB909A-F7E9-4EA0-9712-9D22584A5FF7}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -3310,21 +3307,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>561</v>
@@ -3338,7 +3335,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>624</v>
@@ -3352,7 +3349,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>587</v>
@@ -3366,7 +3363,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>143</v>
@@ -3380,7 +3377,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>142</v>
@@ -3394,7 +3391,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>107</v>
@@ -3408,7 +3405,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>225</v>
@@ -3422,7 +3419,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>501</v>
@@ -3436,7 +3433,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>442</v>
@@ -3450,7 +3447,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>133</v>
@@ -3464,7 +3461,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>76</v>
@@ -3478,7 +3475,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>246</v>
@@ -3492,7 +3489,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>483</v>
@@ -3506,7 +3503,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>34</v>
@@ -3520,7 +3517,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>85</v>
@@ -3534,7 +3531,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>349</v>
@@ -3548,7 +3545,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>87</v>
@@ -3562,7 +3559,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>73</v>
@@ -3576,7 +3573,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>216</v>
@@ -3590,7 +3587,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>135</v>

</xml_diff>